<commit_message>
*fixed missing *12 in sportsExpenditure.R *fixed wrong sign error introduced during overhaul of EEG reforms *income tax only is now really income tax only. Not income tax + soli
</commit_message>
<xml_diff>
--- a/estimates/sportsExpenditure.xlsx
+++ b/estimates/sportsExpenditure.xlsx
@@ -63,13 +63,13 @@
     <t>earnings_effect_high_vs_low</t>
   </si>
   <si>
-    <t>https://ideas.repec.org/p/diw/diwsop/diw_sp1040.html</t>
-  </si>
-  <si>
     <t>Pawlowski et al. (2019) Figure 2 &amp; Text p. 19</t>
   </si>
   <si>
     <t>The authors do not present their estimates in a table with standard errors. Instead they show the effect for each year in Figure 2. The effect is also somewhat jumpy between years.  However, the authors mention in the text what they believe to be the average effect. (i.e. 260€ for men / 0 for women when comparing high to low expenditure). Looking at the graph these appear to be significant at at about 10%.</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/p/usg/econwp/201906.html</t>
   </si>
 </sst>
 </file>
@@ -893,7 +893,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,13 +968,13 @@
         <v>1</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -987,10 +987,7 @@
       <c r="L5" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
* updated papers that have been published in peer reviewed journals * downgraded papers with DiD setups that include plausibly random treatment allocation to 3,3 on the SMS. Papers affected: Dustmann & Schönberg (2012), Collischon et al. (2020), Frodermann et al. (2020), Dolls et al. (2019) * minor adjustments to SMS scores on some other papers * changed p-value in sportsExpenditure.xlsx to 5 percent. The published version shows 95% CI's. And the results are still sig.
</commit_message>
<xml_diff>
--- a/estimates/sportsExpenditure.xlsx
+++ b/estimates/sportsExpenditure.xlsx
@@ -63,13 +63,13 @@
     <t>earnings_effect_high_vs_low</t>
   </si>
   <si>
-    <t>Pawlowski et al. (2019) Figure 2 &amp; Text p. 19</t>
-  </si>
-  <si>
-    <t>The authors do not present their estimates in a table with standard errors. Instead they show the effect for each year in Figure 2. The effect is also somewhat jumpy between years.  However, the authors mention in the text what they believe to be the average effect. (i.e. 260€ for men / 0 for women when comparing high to low expenditure). Looking at the graph these appear to be significant at at about 10%.</t>
-  </si>
-  <si>
     <t>https://ideas.repec.org/p/usg/econwp/201906.html</t>
+  </si>
+  <si>
+    <t>Pawlowski et al. (2019) Figure 2 &amp; Text p. 19, Figure 5 of the published version</t>
+  </si>
+  <si>
+    <t>The authors do not present their estimates in a table with standard errors. Instead they show the effect for each year in Figure 2. The effect is also somewhat jumpy between years.  However, the authors mention in the text what they believe to be the average effect. (i.e. 260€ for men / 0 for women when comparing high to low expenditure). Looking at the graph these appear to be significant at at about 5%. The results appear to be unchanged in the version that was published in Labor Economics in 2021.</t>
   </si>
 </sst>
 </file>
@@ -893,7 +893,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -954,7 +954,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -962,19 +962,19 @@
         <v>260</v>
       </c>
       <c r="E2">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="J2">
         <v>1</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>